<commit_message>
Test case 522 modified
</commit_message>
<xml_diff>
--- a/test_files/Code_list_version2.xlsx
+++ b/test_files/Code_list_version2.xlsx
@@ -12,50 +12,95 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="61">
   <si>
     <t>CODEVALUE</t>
   </si>
   <si>
+    <t>ORGANIZATION</t>
+  </si>
+  <si>
+    <t>INFORMATIONDOMAIN</t>
+  </si>
+  <si>
+    <t>VERSION</t>
+  </si>
+  <si>
+    <t>STATUS</t>
+  </si>
+  <si>
+    <t>PREFLABEL_FI</t>
+  </si>
+  <si>
+    <t>PREFLABEL_SV</t>
+  </si>
+  <si>
+    <t>PREFLABEL_EN</t>
+  </si>
+  <si>
+    <t>DEFINITION_FI</t>
+  </si>
+  <si>
+    <t>DEFINITION_SV</t>
+  </si>
+  <si>
+    <t>DEFINITION_EN</t>
+  </si>
+  <si>
+    <t>DESCRIPTION_FI</t>
+  </si>
+  <si>
+    <t>DESCRIPTION_SV</t>
+  </si>
+  <si>
+    <t>DESCRIPTION_EN</t>
+  </si>
+  <si>
+    <t>CHANGENOTE_FI</t>
+  </si>
+  <si>
+    <t>CHANGENOTE_SV</t>
+  </si>
+  <si>
+    <t>CHANGENOTE_EN</t>
+  </si>
+  <si>
+    <t>STARTDATE</t>
+  </si>
+  <si>
+    <t>ENDDATE</t>
+  </si>
+  <si>
+    <t>SOURCE</t>
+  </si>
+  <si>
+    <t>LEGALBASE</t>
+  </si>
+  <si>
+    <t>GOVERNANCEPOLICY</t>
+  </si>
+  <si>
+    <t>LICENSE</t>
+  </si>
+  <si>
+    <t>Koodisto7001</t>
+  </si>
+  <si>
+    <t>74a41211-8c99-4835-a519-7a61612b1098</t>
+  </si>
+  <si>
     <t>BROADER</t>
   </si>
   <si>
     <t>ID</t>
   </si>
   <si>
-    <t>STATUS</t>
-  </si>
-  <si>
     <t>HIERARCHYLEVEL</t>
   </si>
   <si>
-    <t>PREFLABEL_FI</t>
-  </si>
-  <si>
-    <t>PREFLABEL_SV</t>
-  </si>
-  <si>
-    <t>PREFLABEL_EN</t>
-  </si>
-  <si>
-    <t>DESCRIPTION_FI</t>
-  </si>
-  <si>
-    <t>DESCRIPTION_SV</t>
-  </si>
-  <si>
-    <t>DESCRIPTION_EN</t>
-  </si>
-  <si>
     <t>SHORTNAME_FI</t>
   </si>
   <si>
-    <t>STARTDATE</t>
-  </si>
-  <si>
-    <t>ENDDATE</t>
-  </si>
-  <si>
     <t>testikoodi01</t>
   </si>
   <si>
@@ -65,6 +110,9 @@
     <t>Testikoodi 01</t>
   </si>
   <si>
+    <t>P1;P10;P11</t>
+  </si>
+  <si>
     <t>kuvausFI</t>
   </si>
   <si>
@@ -74,27 +122,42 @@
     <t>lyhytFI</t>
   </si>
   <si>
-    <t>ORGANIZATION</t>
-  </si>
-  <si>
-    <t>INFORMATIONDOMAIN</t>
-  </si>
-  <si>
     <t>testikoodi02</t>
   </si>
   <si>
+    <t>DRAFT</t>
+  </si>
+  <si>
     <t>Testikoodi 02</t>
   </si>
   <si>
+    <t>koodisto7001</t>
+  </si>
+  <si>
+    <t>määritelmäFI</t>
+  </si>
+  <si>
     <t>testikoodi03</t>
   </si>
   <si>
     <t>Testikoodi 03</t>
   </si>
   <si>
+    <t>muutostietoFI</t>
+  </si>
+  <si>
     <t>testikoodi04</t>
   </si>
   <si>
+    <t>lähdeFI</t>
+  </si>
+  <si>
+    <t>lakiperusteFI</t>
+  </si>
+  <si>
+    <t>sitovuustasoFI</t>
+  </si>
+  <si>
     <t>Testikoodi 04</t>
   </si>
   <si>
@@ -119,79 +182,19 @@
     <t>testikoodi08</t>
   </si>
   <si>
-    <t>VERSION</t>
-  </si>
-  <si>
     <t>Testikoodi 08</t>
   </si>
   <si>
     <t>testikoodi09</t>
   </si>
   <si>
-    <t>DEFINITION_FI</t>
-  </si>
-  <si>
-    <t>DEFINITION_SV</t>
-  </si>
-  <si>
     <t>Testikoodi 09</t>
   </si>
   <si>
-    <t>DEFINITION_EN</t>
-  </si>
-  <si>
     <t>testikoodi10</t>
   </si>
   <si>
-    <t>CHANGENOTE_FI</t>
-  </si>
-  <si>
-    <t>CHANGENOTE_SV</t>
-  </si>
-  <si>
     <t>Testikoodi 10</t>
-  </si>
-  <si>
-    <t>CHANGENOTE_EN</t>
-  </si>
-  <si>
-    <t>SOURCE</t>
-  </si>
-  <si>
-    <t>LEGALBASE</t>
-  </si>
-  <si>
-    <t>GOVERNANCEPOLICY</t>
-  </si>
-  <si>
-    <t>LICENSE</t>
-  </si>
-  <si>
-    <t>Koodisto7001</t>
-  </si>
-  <si>
-    <t>74a41211-8c99-4835-a519-7a61612b1098</t>
-  </si>
-  <si>
-    <t>P1;P10;P11</t>
-  </si>
-  <si>
-    <t>koodisto7001</t>
-  </si>
-  <si>
-    <t>määritelmäFI</t>
-  </si>
-  <si>
-    <t>muutostietoFI</t>
-  </si>
-  <si>
-    <t>lähdeFI</t>
-  </si>
-  <si>
-    <t>lakiperusteFI</t>
-  </si>
-  <si>
-    <t>sitovuustasoFI</t>
   </si>
 </sst>
 </file>
@@ -239,14 +242,14 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
@@ -304,16 +307,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>21</v>
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
@@ -325,103 +328,103 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>39</v>
+        <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>41</v>
+        <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="3" t="s">
-        <v>51</v>
+      <c r="A2" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>53</v>
+        <v>24</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="D2" s="5">
         <v>101.0</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>15</v>
+      <c r="E2" s="6" t="s">
+        <v>37</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="M2" s="1"/>
       <c r="N2" s="1" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
-      <c r="R2" s="2">
+      <c r="R2" s="4">
         <v>43161.0</v>
       </c>
-      <c r="S2" s="2">
+      <c r="S2" s="4">
         <v>43189.0</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="W2" s="1"/>
     </row>
@@ -1454,16 +1457,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
@@ -1475,70 +1478,70 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M2" s="2">
+        <v>35</v>
+      </c>
+      <c r="M2" s="4">
         <v>43133.0</v>
       </c>
-      <c r="N2" s="2">
+      <c r="N2" s="4">
         <v>43352.0</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -1551,18 +1554,18 @@
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -1575,16 +1578,16 @@
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -1597,18 +1600,18 @@
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -1621,16 +1624,16 @@
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -1643,18 +1646,18 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -1667,18 +1670,18 @@
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -1691,18 +1694,18 @@
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -1715,18 +1718,18 @@
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>

</xml_diff>